<commit_message>
Lets Beat the GIT...HARDER
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MY FILES\crowdstaffing-team\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBC68AF4-81B9-406D-BD93-0D47C958058B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C216D849-9880-4923-A7B8-EE4C1AE2427C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,9 +25,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>wwrgrthbh eryuo 4tot3ot4</t>
+    <t>egrggerge</t>
+  </si>
+  <si>
+    <t>ergerghog24</t>
+  </si>
+  <si>
+    <t>wrlrgpirhgwp</t>
+  </si>
+  <si>
+    <t>oinohrg3wg</t>
   </si>
 </sst>
 </file>
@@ -345,9 +354,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -356,6 +367,21 @@
         <v>0</v>
       </c>
     </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
I Will Be BACK
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MY FILES\crowdstaffing-team\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C216D849-9880-4923-A7B8-EE4C1AE2427C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27D4DF95-AA4B-440C-AD95-B5C41454572E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
     <t>wrlrgpirhgwp</t>
   </si>
   <si>
-    <t>oinohrg3wg</t>
+    <t>eetgr5g</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
WILL BE BACK AFTER LUNCH
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MY FILES\crowdstaffing-team\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27D4DF95-AA4B-440C-AD95-B5C41454572E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CEE8089-ABF2-47DA-BDE8-9CCDD58D1701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>egrggerge</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>eetgr5g</t>
+  </si>
+  <si>
+    <t>verger</t>
   </si>
 </sst>
 </file>
@@ -354,32 +357,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F13" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
i am back after lunch
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MY FILES\crowdstaffing-team\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CEE8089-ABF2-47DA-BDE8-9CCDD58D1701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38C5E61A-FDEA-4E0D-B575-BF77FA55805E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>egrggerge</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>verger</t>
+  </si>
+  <si>
+    <t>ebe</t>
   </si>
 </sst>
 </file>
@@ -360,7 +363,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -385,6 +388,11 @@
         <v>3</v>
       </c>
     </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F13" t="s">
         <v>4</v>

</xml_diff>